<commit_message>
tilføjet lidt gui til clienten
</commit_message>
<xml_diff>
--- a/iteration mandetimer.xlsx
+++ b/iteration mandetimer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>rasmus</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>parprogrammering</t>
+  </si>
+  <si>
+    <t>storypoint pr time</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,6 +667,14 @@
       </c>
       <c r="C22" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rettet iteration og mandetimer opdateret
</commit_message>
<xml_diff>
--- a/iteration mandetimer.xlsx
+++ b/iteration mandetimer.xlsx
@@ -69,12 +69,6 @@
     <t>lave det brugervenligt</t>
   </si>
   <si>
-    <t>om ugen for alle mand</t>
-  </si>
-  <si>
-    <t>vi har besluttet at tilføj log tager 4 mandedage</t>
-  </si>
-  <si>
     <t>skal ganges med esitimatet på 5 point</t>
   </si>
   <si>
@@ -90,7 +84,13 @@
     <t>parprogrammering</t>
   </si>
   <si>
-    <t>storypoint pr time</t>
+    <t>timer om ugen for alle mand</t>
+  </si>
+  <si>
+    <t>vi har besluttet at tilføj log tager 5 mandedage</t>
+  </si>
+  <si>
+    <t>Timer per storypoint</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -144,10 +144,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +464,7 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -477,12 +481,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -501,12 +505,8 @@
       <c r="F4">
         <v>2.75</v>
       </c>
-      <c r="G4">
-        <f>SUM(B4:F4)</f>
-        <v>20.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -525,12 +525,8 @@
       <c r="F5">
         <v>2.75</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G6" si="0">SUM(B5:F5)</f>
-        <v>20.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -549,12 +545,8 @@
       <c r="F6">
         <v>2.75</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>20.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -573,119 +565,157 @@
       <c r="F7">
         <v>2.75</v>
       </c>
-      <c r="G7">
-        <f>SUM(B7:F7)</f>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B4:B7)</f>
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">SUM(C4:C7)</f>
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B8:F8)</f>
+        <v>83</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>83</v>
+      </c>
+      <c r="I12">
+        <f>H12/4</f>
         <v>20.75</v>
       </c>
-      <c r="H7">
-        <f>G7*2</f>
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="1">
-        <f>SUM(G4:G7)</f>
-        <v>83</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <f>(C18/D18)</f>
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2">
-        <f>(C18*E18*4)</f>
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <f>(C19/D19)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f>(C19*E19*4)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <f>(B19/2)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>(B20/2)</f>
         <v>10</v>
       </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>0.5</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>H12/G12</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="C25" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>G12/H12</f>
+        <v>0.24096385542168675</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H8:K8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
startet på sprint 1 indhold
</commit_message>
<xml_diff>
--- a/iteration mandetimer.xlsx
+++ b/iteration mandetimer.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>rasmus</t>
   </si>
@@ -455,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,13 +724,271 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+      <c r="C4">
+        <v>4.5</v>
+      </c>
+      <c r="D4">
+        <v>4.5</v>
+      </c>
+      <c r="E4">
+        <v>4.5</v>
+      </c>
+      <c r="F4">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4.5</v>
+      </c>
+      <c r="C5">
+        <v>4.5</v>
+      </c>
+      <c r="D5">
+        <v>4.5</v>
+      </c>
+      <c r="E5">
+        <v>4.5</v>
+      </c>
+      <c r="F5">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4.5</v>
+      </c>
+      <c r="C6">
+        <v>4.5</v>
+      </c>
+      <c r="D6">
+        <v>4.5</v>
+      </c>
+      <c r="E6">
+        <v>4.5</v>
+      </c>
+      <c r="F6">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4.5</v>
+      </c>
+      <c r="C7">
+        <v>4.5</v>
+      </c>
+      <c r="D7">
+        <v>4.5</v>
+      </c>
+      <c r="E7">
+        <v>4.5</v>
+      </c>
+      <c r="F7">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B4:B7)</f>
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:F8" si="0">SUM(C4:C7)</f>
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B8:F8)</f>
+        <v>83</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>83</v>
+      </c>
+      <c r="I12">
+        <f>H12/4</f>
+        <v>20.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f>(C19/D19)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f>(C19*E19*4)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f>(B20/2)</f>
+        <v>12.5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>H12/G12</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>G12/H12</f>
+        <v>0.24096385542168675</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H8:K8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -743,4 +1002,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>